<commit_message>
Tách time login ra bảng riêng
</commit_message>
<xml_diff>
--- a/ToolBaoCao/App_Data/DM_COSOKCB.xlsx
+++ b/ToolBaoCao/App_Data/DM_COSOKCB.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chuongnv.laocai\Documents\Zalo Received Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Private\AChuong\ToolBaoCao\ToolBaoCao\App_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCDE8F5B-D1A4-4F59-A5E4-7023B4D9E65E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DM_COSOKCB" sheetId="1" r:id="rId1"/>
@@ -1962,7 +1963,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2289,13 +2290,13 @@
   </cellStyleXfs>
   <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="49" fontId="5" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2304,7 +2305,7 @@
     <xf numFmtId="49" fontId="6" fillId="7" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="49" fontId="8" fillId="9" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2313,10 +2314,10 @@
     <xf numFmtId="3" fontId="9" fillId="10" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="49" fontId="12" fillId="13" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2325,17 +2326,17 @@
     <xf numFmtId="49" fontId="13" fillId="14" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
@@ -2345,10 +2346,10 @@
     <xf numFmtId="3" fontId="9" fillId="15" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
   </cellXfs>
@@ -2630,11 +2631,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AG177"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="T1" workbookViewId="0">
-      <selection activeCell="AG1" sqref="AG1:AG16"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="AD9" sqref="AD9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
điều chỉnh tròn số /bcTuan/createBCTuan
</commit_message>
<xml_diff>
--- a/ToolBaoCao/App_Data/DM_COSOKCB.xlsx
+++ b/ToolBaoCao/App_Data/DM_COSOKCB.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Private\AChuong\ToolBaoCao\ToolBaoCao\App_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCDE8F5B-D1A4-4F59-A5E4-7023B4D9E65E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF05189D-0DD2-4051-93ED-DE6E6D05C44B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DM_COSOKCB" sheetId="1" r:id="rId1"/>
@@ -2634,7 +2634,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AG177"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <selection activeCell="AD9" sqref="AD9"/>
     </sheetView>
   </sheetViews>

</xml_diff>